<commit_message>
test new api with numbers and tcam
</commit_message>
<xml_diff>
--- a/entry_lists/Sonoma Provisional Entry List.xlsx
+++ b/entry_lists/Sonoma Provisional Entry List.xlsx
@@ -7504,10 +7504,8 @@
           <t>GT America</t>
         </is>
       </c>
-      <c r="B7" s="398" t="inlineStr">
-        <is>
-          <t>333</t>
-        </is>
+      <c r="B7" s="398" t="n">
+        <v>333</v>
       </c>
       <c r="C7" s="399" t="inlineStr">
         <is>
@@ -7553,10 +7551,8 @@
           <t>GT America</t>
         </is>
       </c>
-      <c r="B8" s="403" t="inlineStr">
-        <is>
-          <t>222</t>
-        </is>
+      <c r="B8" s="403" t="n">
+        <v>222</v>
       </c>
       <c r="C8" s="404" t="inlineStr">
         <is>
@@ -7598,10 +7594,8 @@
           <t>GT America</t>
         </is>
       </c>
-      <c r="B9" s="406" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="B9" s="406" t="n">
+        <v>2</v>
       </c>
       <c r="C9" s="407" t="inlineStr">
         <is>
@@ -8390,10 +8384,8 @@
           <t>TC America</t>
         </is>
       </c>
-      <c r="B7" s="478" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
+      <c r="B7" s="478" t="n">
+        <v>80</v>
       </c>
       <c r="C7" s="479" t="inlineStr">
         <is>
@@ -8439,10 +8431,8 @@
           <t>TC America</t>
         </is>
       </c>
-      <c r="B8" s="482" t="inlineStr">
-        <is>
-          <t>789</t>
-        </is>
+      <c r="B8" s="482" t="n">
+        <v>789</v>
       </c>
       <c r="C8" s="482" t="inlineStr">
         <is>
@@ -8541,10 +8531,8 @@
           <t>TC America</t>
         </is>
       </c>
-      <c r="B9" s="484" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 50</t>
-        </is>
+      <c r="B9" s="484" t="n">
+        <v>50</v>
       </c>
       <c r="C9" s="485" t="inlineStr">
         <is>
@@ -8639,19 +8627,17 @@
           <t>TC America</t>
         </is>
       </c>
-      <c r="B10" s="484" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="B10" s="484" t="n">
+        <v>56</v>
       </c>
       <c r="C10" s="485" t="inlineStr">
         <is>
-          <t>Lone Star Racing</t>
+          <t>Blue Jays Racing</t>
         </is>
       </c>
       <c r="D10" s="486" t="inlineStr">
         <is>
-          <t>Juan Pablo Martinez</t>
+          <t>Roy Halladay</t>
         </is>
       </c>
       <c r="E10" s="486" t="inlineStr">
@@ -8659,19 +8645,15 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="F10" s="488" t="inlineStr">
-        <is>
-          <t>sponsor - test, Im still testing this janky backend</t>
-        </is>
-      </c>
+      <c r="F10" s="488" t="inlineStr"/>
       <c r="G10" s="488" t="inlineStr">
         <is>
-          <t>subaruBrz</t>
+          <t>Honda Civic Type-R TC</t>
         </is>
       </c>
       <c r="H10" s="487" t="inlineStr">
         <is>
-          <t>TCA</t>
+          <t>TC</t>
         </is>
       </c>
       <c r="I10" s="25" t="n"/>
@@ -8741,19 +8723,17 @@
           <t>TC America</t>
         </is>
       </c>
-      <c r="B11" s="489" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="B11" s="489" t="n">
+        <v>9</v>
       </c>
       <c r="C11" s="485" t="inlineStr">
         <is>
-          <t>Skip Barber Racing</t>
+          <t>Lone Star Racing</t>
         </is>
       </c>
       <c r="D11" s="486" t="inlineStr">
         <is>
-          <t>Matt Chapman</t>
+          <t>Juan Pablo Martinez</t>
         </is>
       </c>
       <c r="E11" s="485" t="inlineStr">
@@ -8763,12 +8743,12 @@
       </c>
       <c r="F11" s="485" t="inlineStr">
         <is>
-          <t>Mustaches, BioSteel</t>
+          <t>sponsor - test, Im still testing this janky backend</t>
         </is>
       </c>
       <c r="G11" s="488" t="inlineStr">
         <is>
-          <t>Honda Civic Si</t>
+          <t>subaruBrz</t>
         </is>
       </c>
       <c r="H11" s="487" t="inlineStr">
@@ -8838,14 +8818,44 @@
       <c r="BP11" s="26" t="n"/>
     </row>
     <row r="12" ht="46.75" customFormat="1" customHeight="1" s="10">
-      <c r="A12" s="516" t="n"/>
-      <c r="B12" s="490" t="n"/>
-      <c r="C12" s="490" t="n"/>
-      <c r="D12" s="490" t="n"/>
-      <c r="E12" s="490" t="n"/>
-      <c r="F12" s="490" t="n"/>
-      <c r="G12" s="490" t="n"/>
-      <c r="H12" s="491" t="n"/>
+      <c r="A12" s="516" t="inlineStr">
+        <is>
+          <t>TC America</t>
+        </is>
+      </c>
+      <c r="B12" s="490" t="n">
+        <v>9</v>
+      </c>
+      <c r="C12" s="490" t="inlineStr">
+        <is>
+          <t>Skip Barber Racing</t>
+        </is>
+      </c>
+      <c r="D12" s="490" t="inlineStr">
+        <is>
+          <t>Matt Chapman</t>
+        </is>
+      </c>
+      <c r="E12" s="490" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="F12" s="490" t="inlineStr">
+        <is>
+          <t>Mustaches, BioSteel</t>
+        </is>
+      </c>
+      <c r="G12" s="490" t="inlineStr">
+        <is>
+          <t>Honda Civic Si</t>
+        </is>
+      </c>
+      <c r="H12" s="491" t="inlineStr">
+        <is>
+          <t>TCA</t>
+        </is>
+      </c>
       <c r="I12" s="25" t="n"/>
       <c r="J12" s="25" t="n"/>
       <c r="K12" s="25" t="n"/>

</xml_diff>

<commit_message>
update with new changes for dates
</commit_message>
<xml_diff>
--- a/entry_lists/Sonoma Provisional Entry List.xlsx
+++ b/entry_lists/Sonoma Provisional Entry List.xlsx
@@ -5709,7 +5709,7 @@
     <row r="4" ht="45" customHeight="1">
       <c r="D4" s="530" t="inlineStr">
         <is>
-          <t>April 5 - 7</t>
+          <t>Apr 5-7</t>
         </is>
       </c>
     </row>
@@ -6587,7 +6587,7 @@
     <row r="4" ht="45" customHeight="1">
       <c r="D4" s="530" t="inlineStr">
         <is>
-          <t>April 5 - 7</t>
+          <t>Apr 5-7</t>
         </is>
       </c>
     </row>
@@ -7739,7 +7739,7 @@
     <row r="4" ht="45" customHeight="1">
       <c r="D4" s="527" t="inlineStr">
         <is>
-          <t>April 5 - 7</t>
+          <t>Apr 5-7</t>
         </is>
       </c>
     </row>
@@ -8575,7 +8575,7 @@
     <row r="4" ht="45" customHeight="1">
       <c r="D4" s="527" t="inlineStr">
         <is>
-          <t>April 5 - 7</t>
+          <t>Apr 5-7</t>
         </is>
       </c>
     </row>
@@ -10875,7 +10875,7 @@
     <row r="4" ht="63" customHeight="1">
       <c r="D4" s="529" t="inlineStr">
         <is>
-          <t>April 5 - 7</t>
+          <t>Apr 5-7</t>
         </is>
       </c>
       <c r="I4" s="528" t="n"/>

</xml_diff>

<commit_message>
change name of functions folder to utility, udpate imports
</commit_message>
<xml_diff>
--- a/entry_lists/Sonoma Provisional Entry List.xlsx
+++ b/entry_lists/Sonoma Provisional Entry List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GTWCA" sheetId="1" state="visible" r:id="rId1"/>
@@ -3169,6 +3169,9 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3186,9 +3189,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -5087,6 +5087,47 @@
     </pic>
     <clientData/>
   </twoCellAnchor>
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>142875</rowOff>
+    </from>
+    <to>
+      <col>13</col>
+      <colOff>866775</colOff>
+      <row>3</row>
+      <rowOff>492125</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Picture 4"/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="15033625" y="333375"/>
+          <a:ext cx="3581400" cy="1492250"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
 </wsDr>
 </file>
 
@@ -5122,6 +5163,47 @@
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="143565" y="552173"/>
           <a:ext cx="3990817" cy="940077"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>12</col>
+      <colOff>95250</colOff>
+      <row>1</row>
+      <rowOff>142875</rowOff>
+    </from>
+    <to>
+      <col>13</col>
+      <colOff>660400</colOff>
+      <row>3</row>
+      <rowOff>492125</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Picture 1"/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="15478125" y="333375"/>
+          <a:ext cx="3581400" cy="1492250"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
@@ -5179,6 +5261,47 @@
     </pic>
     <clientData/>
   </twoCellAnchor>
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>8</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>79375</rowOff>
+    </from>
+    <to>
+      <col>10</col>
+      <colOff>41275</colOff>
+      <row>3</row>
+      <rowOff>428625</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Picture 2"/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="13081000" y="269875"/>
+          <a:ext cx="3581400" cy="1492250"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
 </wsDr>
 </file>
 
@@ -5225,6 +5348,47 @@
     </pic>
     <clientData/>
   </twoCellAnchor>
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>6</col>
+      <colOff>285751</colOff>
+      <row>1</row>
+      <rowOff>206375</rowOff>
+    </from>
+    <to>
+      <col>7</col>
+      <colOff>783134</colOff>
+      <row>3</row>
+      <rowOff>553847</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Picture 3"/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="12446001" y="396875"/>
+          <a:ext cx="3577133" cy="1490472"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
 </wsDr>
 </file>
 
@@ -5260,6 +5424,47 @@
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="222250" y="1092200"/>
           <a:ext cx="3251200" cy="1168400"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>5</col>
+      <colOff>1651000</colOff>
+      <row>1</row>
+      <rowOff>746125</rowOff>
+    </from>
+    <to>
+      <col>8</col>
+      <colOff>200025</colOff>
+      <row>3</row>
+      <rowOff>396875</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Picture 3"/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="8096250" y="936625"/>
+          <a:ext cx="3581400" cy="1492250"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
@@ -5668,8 +5873,8 @@
   </sheetPr>
   <dimension ref="A2:X34"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="80" zoomScaleNormal="90" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" view="pageLayout" zoomScale="80" zoomScaleNormal="90" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15"/>
@@ -5692,7 +5897,7 @@
   <sheetData>
     <row r="2" ht="45" customHeight="1">
       <c r="A2" s="523" t="n"/>
-      <c r="D2" s="530" t="inlineStr">
+      <c r="D2" s="524" t="inlineStr">
         <is>
           <t>Sonoma Raceway</t>
         </is>
@@ -5700,14 +5905,14 @@
       <c r="M2" s="523" t="n"/>
     </row>
     <row r="3" ht="45" customHeight="1">
-      <c r="D3" s="524" t="inlineStr">
+      <c r="D3" s="525" t="inlineStr">
         <is>
           <t>Provisional Entry List</t>
         </is>
       </c>
     </row>
     <row r="4" ht="45" customHeight="1">
-      <c r="D4" s="530" t="inlineStr">
+      <c r="D4" s="524" t="inlineStr">
         <is>
           <t>Apr 5-7</t>
         </is>
@@ -5881,7 +6086,7 @@
       <c r="L7" s="230" t="inlineStr"/>
       <c r="M7" s="230" t="inlineStr">
         <is>
-          <t>acuraNsxGt3Evo22</t>
+          <t>Acura NSX GT3 EVO22</t>
         </is>
       </c>
       <c r="N7" s="231" t="inlineStr">
@@ -6163,7 +6368,7 @@
       <c r="I15" s="259" t="n"/>
       <c r="J15" s="259" t="n"/>
       <c r="K15" s="259" t="n"/>
-      <c r="L15" s="528" t="n"/>
+      <c r="L15" s="529" t="n"/>
       <c r="M15" s="116" t="n"/>
       <c r="N15" s="272" t="n"/>
       <c r="R15" s="273" t="n"/>
@@ -6548,7 +6753,7 @@
   <dimension ref="A2:Y40"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="80" zoomScaleNormal="115" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15"/>
@@ -6569,30 +6774,30 @@
   </cols>
   <sheetData>
     <row r="2" ht="45" customHeight="1">
-      <c r="A2" s="525" t="n"/>
-      <c r="D2" s="530" t="inlineStr">
+      <c r="A2" s="526" t="n"/>
+      <c r="D2" s="524" t="inlineStr">
         <is>
           <t>Sonoma Raceway</t>
         </is>
       </c>
-      <c r="M2" s="525" t="n"/>
+      <c r="M2" s="526" t="n"/>
     </row>
     <row r="3" ht="45" customHeight="1">
-      <c r="D3" s="524" t="inlineStr">
+      <c r="D3" s="525" t="inlineStr">
         <is>
           <t>Provisional Entry List</t>
         </is>
       </c>
     </row>
     <row r="4" ht="45" customHeight="1">
-      <c r="D4" s="530" t="inlineStr">
+      <c r="D4" s="524" t="inlineStr">
         <is>
           <t>Apr 5-7</t>
         </is>
       </c>
     </row>
     <row r="5" ht="16" customHeight="1" thickBot="1">
-      <c r="R5" s="526" t="inlineStr">
+      <c r="R5" s="527" t="inlineStr">
         <is>
           <t>Admin Checks</t>
         </is>
@@ -6765,7 +6970,7 @@
       <c r="L7" s="216" t="inlineStr"/>
       <c r="M7" s="217" t="inlineStr">
         <is>
-          <t>nissanZGt4</t>
+          <t>Nissan Z GT4</t>
         </is>
       </c>
       <c r="N7" s="217" t="inlineStr">
@@ -7701,7 +7906,7 @@
   <dimension ref="A2:R41"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="80" zoomScaleNormal="90" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:H4"/>
+      <selection activeCell="I2" sqref="I2:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15"/>
@@ -7721,30 +7926,30 @@
   </cols>
   <sheetData>
     <row r="2" ht="45" customHeight="1">
-      <c r="A2" s="525" t="n"/>
-      <c r="D2" s="527" t="inlineStr">
+      <c r="A2" s="526" t="n"/>
+      <c r="D2" s="528" t="inlineStr">
         <is>
           <t>Sonoma Raceway</t>
         </is>
       </c>
-      <c r="I2" s="525" t="n"/>
+      <c r="I2" s="526" t="n"/>
     </row>
     <row r="3" ht="45" customHeight="1">
-      <c r="D3" s="527" t="inlineStr">
+      <c r="D3" s="528" t="inlineStr">
         <is>
           <t>Provisional Entry List</t>
         </is>
       </c>
     </row>
     <row r="4" ht="45" customHeight="1">
-      <c r="D4" s="527" t="inlineStr">
+      <c r="D4" s="528" t="inlineStr">
         <is>
           <t>Apr 5-7</t>
         </is>
       </c>
     </row>
     <row r="5" ht="16" customHeight="1" thickBot="1">
-      <c r="N5" s="525" t="inlineStr">
+      <c r="N5" s="526" t="inlineStr">
         <is>
           <t>Admin Checks</t>
         </is>
@@ -8538,7 +8743,7 @@
   <dimension ref="A2:BP36"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="80" zoomScaleNormal="70" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:F3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15"/>
@@ -8557,30 +8762,30 @@
   </cols>
   <sheetData>
     <row r="2" ht="45" customHeight="1">
-      <c r="A2" s="525" t="n"/>
-      <c r="D2" s="527" t="inlineStr">
+      <c r="A2" s="526" t="n"/>
+      <c r="D2" s="528" t="inlineStr">
         <is>
           <t>Sonoma Raceway</t>
         </is>
       </c>
-      <c r="G2" s="525" t="n"/>
+      <c r="G2" s="526" t="n"/>
     </row>
     <row r="3" ht="45" customHeight="1">
-      <c r="D3" s="527" t="inlineStr">
+      <c r="D3" s="528" t="inlineStr">
         <is>
           <t>Provisional Entry List</t>
         </is>
       </c>
     </row>
     <row r="4" ht="45" customHeight="1">
-      <c r="D4" s="527" t="inlineStr">
+      <c r="D4" s="528" t="inlineStr">
         <is>
           <t>Apr 5-7</t>
         </is>
       </c>
     </row>
     <row r="5" ht="16" customHeight="1" thickBot="1">
-      <c r="L5" s="525" t="inlineStr">
+      <c r="L5" s="526" t="inlineStr">
         <is>
           <t>Admin Checks</t>
         </is>
@@ -8790,7 +8995,7 @@
       </c>
       <c r="G8" s="444" t="inlineStr">
         <is>
-          <t>acuraIntegraTypeS</t>
+          <t>Acura Integra Type S</t>
         </is>
       </c>
       <c r="H8" s="445" t="inlineStr">
@@ -9082,7 +9287,7 @@
       </c>
       <c r="G11" s="450" t="inlineStr">
         <is>
-          <t>subaruBrz</t>
+          <t>Subaru BRZ</t>
         </is>
       </c>
       <c r="H11" s="449" t="inlineStr">
@@ -10794,7 +10999,7 @@
   <dimension ref="A1:T42"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:F2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -10817,101 +11022,101 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="528" t="n"/>
+      <c r="A1" s="529" t="n"/>
       <c r="B1" s="16" t="n"/>
       <c r="C1" s="16" t="n"/>
       <c r="D1" s="16" t="n"/>
       <c r="E1" s="16" t="n"/>
       <c r="F1" s="16" t="n"/>
-      <c r="G1" s="528" t="n"/>
-      <c r="H1" s="528" t="n"/>
-      <c r="I1" s="528" t="n"/>
-      <c r="J1" s="528" t="n"/>
-      <c r="K1" s="528" t="n"/>
-      <c r="L1" s="528" t="n"/>
-      <c r="M1" s="528" t="n"/>
-      <c r="N1" s="528" t="n"/>
+      <c r="G1" s="529" t="n"/>
+      <c r="H1" s="529" t="n"/>
+      <c r="I1" s="529" t="n"/>
+      <c r="J1" s="529" t="n"/>
+      <c r="K1" s="529" t="n"/>
+      <c r="L1" s="529" t="n"/>
+      <c r="M1" s="529" t="n"/>
+      <c r="N1" s="529" t="n"/>
     </row>
     <row r="2" ht="73.5" customHeight="1">
-      <c r="A2" s="528" t="n"/>
-      <c r="D2" s="529" t="inlineStr">
+      <c r="A2" s="529" t="n"/>
+      <c r="D2" s="530" t="inlineStr">
         <is>
           <t>Sonoma Raceway</t>
         </is>
       </c>
-      <c r="G2" s="528" t="n"/>
-      <c r="I2" s="528" t="n"/>
-      <c r="J2" s="528" t="n"/>
-      <c r="K2" s="528" t="n"/>
-      <c r="L2" s="528" t="n"/>
-      <c r="M2" s="528" t="n"/>
-      <c r="N2" s="528" t="n"/>
-      <c r="O2" s="528" t="n"/>
-      <c r="P2" s="528" t="n"/>
-      <c r="Q2" s="528" t="n"/>
-      <c r="R2" s="528" t="n"/>
-      <c r="S2" s="528" t="n"/>
-      <c r="T2" s="528" t="n"/>
+      <c r="G2" s="529" t="n"/>
+      <c r="I2" s="529" t="n"/>
+      <c r="J2" s="529" t="n"/>
+      <c r="K2" s="529" t="n"/>
+      <c r="L2" s="529" t="n"/>
+      <c r="M2" s="529" t="n"/>
+      <c r="N2" s="529" t="n"/>
+      <c r="O2" s="529" t="n"/>
+      <c r="P2" s="529" t="n"/>
+      <c r="Q2" s="529" t="n"/>
+      <c r="R2" s="529" t="n"/>
+      <c r="S2" s="529" t="n"/>
+      <c r="T2" s="529" t="n"/>
     </row>
     <row r="3" ht="73.5" customHeight="1">
-      <c r="D3" s="529" t="inlineStr">
+      <c r="D3" s="530" t="inlineStr">
         <is>
           <t>Provisional Entry List</t>
         </is>
       </c>
-      <c r="I3" s="528" t="n"/>
-      <c r="J3" s="528" t="n"/>
-      <c r="K3" s="528" t="n"/>
-      <c r="L3" s="528" t="n"/>
-      <c r="M3" s="528" t="n"/>
-      <c r="N3" s="528" t="n"/>
-      <c r="O3" s="528" t="n"/>
-      <c r="P3" s="528" t="n"/>
-      <c r="Q3" s="528" t="n"/>
-      <c r="R3" s="528" t="n"/>
-      <c r="S3" s="528" t="n"/>
-      <c r="T3" s="528" t="n"/>
+      <c r="I3" s="529" t="n"/>
+      <c r="J3" s="529" t="n"/>
+      <c r="K3" s="529" t="n"/>
+      <c r="L3" s="529" t="n"/>
+      <c r="M3" s="529" t="n"/>
+      <c r="N3" s="529" t="n"/>
+      <c r="O3" s="529" t="n"/>
+      <c r="P3" s="529" t="n"/>
+      <c r="Q3" s="529" t="n"/>
+      <c r="R3" s="529" t="n"/>
+      <c r="S3" s="529" t="n"/>
+      <c r="T3" s="529" t="n"/>
     </row>
     <row r="4" ht="63" customHeight="1">
-      <c r="D4" s="529" t="inlineStr">
+      <c r="D4" s="530" t="inlineStr">
         <is>
           <t>Apr 5-7</t>
         </is>
       </c>
-      <c r="I4" s="528" t="n"/>
-      <c r="J4" s="528" t="n"/>
-      <c r="K4" s="528" t="n"/>
-      <c r="L4" s="528" t="n"/>
-      <c r="M4" s="528" t="n"/>
-      <c r="N4" s="528" t="n"/>
-      <c r="O4" s="528" t="n"/>
-      <c r="P4" s="528" t="n"/>
-      <c r="Q4" s="528" t="n"/>
-      <c r="R4" s="528" t="n"/>
-      <c r="S4" s="528" t="n"/>
-      <c r="T4" s="528" t="n"/>
+      <c r="I4" s="529" t="n"/>
+      <c r="J4" s="529" t="n"/>
+      <c r="K4" s="529" t="n"/>
+      <c r="L4" s="529" t="n"/>
+      <c r="M4" s="529" t="n"/>
+      <c r="N4" s="529" t="n"/>
+      <c r="O4" s="529" t="n"/>
+      <c r="P4" s="529" t="n"/>
+      <c r="Q4" s="529" t="n"/>
+      <c r="R4" s="529" t="n"/>
+      <c r="S4" s="529" t="n"/>
+      <c r="T4" s="529" t="n"/>
     </row>
     <row r="5" ht="15" customHeight="1" thickBot="1">
-      <c r="A5" s="528" t="n"/>
-      <c r="B5" s="528" t="n"/>
+      <c r="A5" s="529" t="n"/>
+      <c r="B5" s="529" t="n"/>
       <c r="C5" s="18" t="n"/>
-      <c r="D5" s="528" t="n"/>
-      <c r="E5" s="528" t="n"/>
-      <c r="F5" s="528" t="n"/>
-      <c r="G5" s="528" t="n"/>
-      <c r="H5" s="528" t="n"/>
-      <c r="I5" s="528" t="n"/>
-      <c r="J5" s="528" t="n"/>
-      <c r="K5" s="528" t="n"/>
-      <c r="L5" s="528" t="n"/>
-      <c r="M5" s="528" t="n"/>
-      <c r="N5" s="528" t="n"/>
-      <c r="O5" s="528" t="n"/>
-      <c r="P5" s="528" t="n"/>
-      <c r="Q5" s="528" t="n"/>
-      <c r="R5" s="528" t="n"/>
-      <c r="S5" s="528" t="n"/>
-      <c r="T5" s="528" t="n"/>
+      <c r="D5" s="529" t="n"/>
+      <c r="E5" s="529" t="n"/>
+      <c r="F5" s="529" t="n"/>
+      <c r="G5" s="529" t="n"/>
+      <c r="H5" s="529" t="n"/>
+      <c r="I5" s="529" t="n"/>
+      <c r="J5" s="529" t="n"/>
+      <c r="K5" s="529" t="n"/>
+      <c r="L5" s="529" t="n"/>
+      <c r="M5" s="529" t="n"/>
+      <c r="N5" s="529" t="n"/>
+      <c r="O5" s="529" t="n"/>
+      <c r="P5" s="529" t="n"/>
+      <c r="Q5" s="529" t="n"/>
+      <c r="R5" s="529" t="n"/>
+      <c r="S5" s="529" t="n"/>
+      <c r="T5" s="529" t="n"/>
     </row>
     <row r="6" ht="33" customHeight="1" thickBot="1">
       <c r="A6" s="360" t="inlineStr">
@@ -10980,12 +11185,12 @@
           <t>Drv Weight</t>
         </is>
       </c>
-      <c r="O6" s="528" t="n"/>
-      <c r="P6" s="528" t="n"/>
-      <c r="Q6" s="528" t="n"/>
-      <c r="R6" s="528" t="n"/>
-      <c r="S6" s="528" t="n"/>
-      <c r="T6" s="528" t="n"/>
+      <c r="O6" s="529" t="n"/>
+      <c r="P6" s="529" t="n"/>
+      <c r="Q6" s="529" t="n"/>
+      <c r="R6" s="529" t="n"/>
+      <c r="S6" s="529" t="n"/>
+      <c r="T6" s="529" t="n"/>
     </row>
     <row r="7" ht="30" customHeight="1" thickTop="1">
       <c r="A7" s="519" t="inlineStr">
@@ -11032,12 +11237,12 @@
       <c r="L7" s="13" t="n"/>
       <c r="M7" s="13" t="n"/>
       <c r="N7" s="13" t="n"/>
-      <c r="O7" s="528" t="n"/>
-      <c r="P7" s="528" t="n"/>
-      <c r="Q7" s="528" t="n"/>
-      <c r="R7" s="528" t="n"/>
-      <c r="S7" s="528" t="n"/>
-      <c r="T7" s="528" t="n"/>
+      <c r="O7" s="529" t="n"/>
+      <c r="P7" s="529" t="n"/>
+      <c r="Q7" s="529" t="n"/>
+      <c r="R7" s="529" t="n"/>
+      <c r="S7" s="529" t="n"/>
+      <c r="T7" s="529" t="n"/>
     </row>
     <row r="8" ht="27" customHeight="1">
       <c r="A8" s="520" t="inlineStr">
@@ -11096,12 +11301,12 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="O8" s="528" t="n"/>
-      <c r="P8" s="528" t="n"/>
-      <c r="Q8" s="528" t="n"/>
-      <c r="R8" s="528" t="n"/>
-      <c r="S8" s="528" t="n"/>
-      <c r="T8" s="528" t="n"/>
+      <c r="O8" s="529" t="n"/>
+      <c r="P8" s="529" t="n"/>
+      <c r="Q8" s="529" t="n"/>
+      <c r="R8" s="529" t="n"/>
+      <c r="S8" s="529" t="n"/>
+      <c r="T8" s="529" t="n"/>
     </row>
     <row r="9" ht="27" customHeight="1">
       <c r="A9" s="520" t="n"/>
@@ -11118,12 +11323,12 @@
       <c r="L9" s="13" t="n"/>
       <c r="M9" s="13" t="n"/>
       <c r="N9" s="13" t="n"/>
-      <c r="O9" s="528" t="n"/>
-      <c r="P9" s="528" t="n"/>
-      <c r="Q9" s="528" t="n"/>
-      <c r="R9" s="528" t="n"/>
-      <c r="S9" s="528" t="n"/>
-      <c r="T9" s="528" t="n"/>
+      <c r="O9" s="529" t="n"/>
+      <c r="P9" s="529" t="n"/>
+      <c r="Q9" s="529" t="n"/>
+      <c r="R9" s="529" t="n"/>
+      <c r="S9" s="529" t="n"/>
+      <c r="T9" s="529" t="n"/>
     </row>
     <row r="10" ht="30" customHeight="1">
       <c r="A10" s="520" t="n"/>
@@ -11168,12 +11373,12 @@
       <c r="L11" s="13" t="n"/>
       <c r="M11" s="13" t="n"/>
       <c r="N11" s="13" t="n"/>
-      <c r="O11" s="528" t="n"/>
-      <c r="P11" s="528" t="n"/>
-      <c r="Q11" s="528" t="n"/>
-      <c r="R11" s="528" t="n"/>
-      <c r="S11" s="528" t="n"/>
-      <c r="T11" s="528" t="n"/>
+      <c r="O11" s="529" t="n"/>
+      <c r="P11" s="529" t="n"/>
+      <c r="Q11" s="529" t="n"/>
+      <c r="R11" s="529" t="n"/>
+      <c r="S11" s="529" t="n"/>
+      <c r="T11" s="529" t="n"/>
     </row>
     <row r="12" ht="27" customHeight="1">
       <c r="A12" s="520" t="n"/>
@@ -11182,7 +11387,11 @@
       <c r="D12" s="28" t="n"/>
       <c r="E12" s="111" t="n"/>
       <c r="F12" s="111" t="n"/>
-      <c r="G12" s="28" t="n"/>
+      <c r="G12" s="28" t="inlineStr">
+        <is>
+          <t>`</t>
+        </is>
+      </c>
       <c r="H12" s="352" t="n"/>
       <c r="I12" s="20" t="n"/>
       <c r="J12" s="21" t="n"/>
@@ -11190,12 +11399,12 @@
       <c r="L12" s="13" t="n"/>
       <c r="M12" s="13" t="n"/>
       <c r="N12" s="13" t="n"/>
-      <c r="O12" s="528" t="n"/>
-      <c r="P12" s="528" t="n"/>
-      <c r="Q12" s="528" t="n"/>
-      <c r="R12" s="528" t="n"/>
-      <c r="S12" s="528" t="n"/>
-      <c r="T12" s="528" t="n"/>
+      <c r="O12" s="529" t="n"/>
+      <c r="P12" s="529" t="n"/>
+      <c r="Q12" s="529" t="n"/>
+      <c r="R12" s="529" t="n"/>
+      <c r="S12" s="529" t="n"/>
+      <c r="T12" s="529" t="n"/>
     </row>
     <row r="13" ht="27" customHeight="1">
       <c r="A13" s="520" t="n"/>
@@ -11212,12 +11421,12 @@
       <c r="L13" s="13" t="n"/>
       <c r="M13" s="13" t="n"/>
       <c r="N13" s="13" t="n"/>
-      <c r="O13" s="528" t="n"/>
-      <c r="P13" s="528" t="n"/>
-      <c r="Q13" s="528" t="n"/>
-      <c r="R13" s="528" t="n"/>
-      <c r="S13" s="528" t="n"/>
-      <c r="T13" s="528" t="n"/>
+      <c r="O13" s="529" t="n"/>
+      <c r="P13" s="529" t="n"/>
+      <c r="Q13" s="529" t="n"/>
+      <c r="R13" s="529" t="n"/>
+      <c r="S13" s="529" t="n"/>
+      <c r="T13" s="529" t="n"/>
     </row>
     <row r="14" ht="27" customHeight="1">
       <c r="A14" s="520" t="n"/>
@@ -11234,12 +11443,12 @@
       <c r="L14" s="13" t="n"/>
       <c r="M14" s="13" t="n"/>
       <c r="N14" s="13" t="n"/>
-      <c r="O14" s="528" t="n"/>
-      <c r="P14" s="528" t="n"/>
-      <c r="Q14" s="528" t="n"/>
-      <c r="R14" s="528" t="n"/>
-      <c r="S14" s="528" t="n"/>
-      <c r="T14" s="528" t="n"/>
+      <c r="O14" s="529" t="n"/>
+      <c r="P14" s="529" t="n"/>
+      <c r="Q14" s="529" t="n"/>
+      <c r="R14" s="529" t="n"/>
+      <c r="S14" s="529" t="n"/>
+      <c r="T14" s="529" t="n"/>
     </row>
     <row r="15" ht="27" customHeight="1">
       <c r="A15" s="520" t="n"/>
@@ -11256,12 +11465,12 @@
       <c r="L15" s="13" t="n"/>
       <c r="M15" s="13" t="n"/>
       <c r="N15" s="13" t="n"/>
-      <c r="O15" s="528" t="n"/>
-      <c r="P15" s="528" t="n"/>
-      <c r="Q15" s="528" t="n"/>
-      <c r="R15" s="528" t="n"/>
-      <c r="S15" s="528" t="n"/>
-      <c r="T15" s="528" t="n"/>
+      <c r="O15" s="529" t="n"/>
+      <c r="P15" s="529" t="n"/>
+      <c r="Q15" s="529" t="n"/>
+      <c r="R15" s="529" t="n"/>
+      <c r="S15" s="529" t="n"/>
+      <c r="T15" s="529" t="n"/>
     </row>
     <row r="16" ht="30" customHeight="1">
       <c r="A16" s="520" t="n"/>
@@ -11293,12 +11502,12 @@
       <c r="L17" s="13" t="n"/>
       <c r="M17" s="13" t="n"/>
       <c r="N17" s="13" t="n"/>
-      <c r="O17" s="528" t="n"/>
-      <c r="P17" s="528" t="n"/>
-      <c r="Q17" s="528" t="n"/>
-      <c r="R17" s="528" t="n"/>
-      <c r="S17" s="528" t="n"/>
-      <c r="T17" s="528" t="n"/>
+      <c r="O17" s="529" t="n"/>
+      <c r="P17" s="529" t="n"/>
+      <c r="Q17" s="529" t="n"/>
+      <c r="R17" s="529" t="n"/>
+      <c r="S17" s="529" t="n"/>
+      <c r="T17" s="529" t="n"/>
     </row>
     <row r="18" ht="30" customHeight="1">
       <c r="A18" s="520" t="n"/>
@@ -11330,12 +11539,12 @@
       <c r="L19" s="13" t="n"/>
       <c r="M19" s="13" t="n"/>
       <c r="N19" s="13" t="n"/>
-      <c r="O19" s="528" t="n"/>
-      <c r="P19" s="528" t="n"/>
-      <c r="Q19" s="528" t="n"/>
-      <c r="R19" s="528" t="n"/>
-      <c r="S19" s="528" t="n"/>
-      <c r="T19" s="528" t="n"/>
+      <c r="O19" s="529" t="n"/>
+      <c r="P19" s="529" t="n"/>
+      <c r="Q19" s="529" t="n"/>
+      <c r="R19" s="529" t="n"/>
+      <c r="S19" s="529" t="n"/>
+      <c r="T19" s="529" t="n"/>
     </row>
     <row r="20" ht="27" customHeight="1">
       <c r="A20" s="520" t="n"/>
@@ -11352,12 +11561,12 @@
       <c r="L20" s="13" t="n"/>
       <c r="M20" s="13" t="n"/>
       <c r="N20" s="13" t="n"/>
-      <c r="O20" s="528" t="n"/>
-      <c r="P20" s="528" t="n"/>
-      <c r="Q20" s="528" t="n"/>
-      <c r="R20" s="528" t="n"/>
-      <c r="S20" s="528" t="n"/>
-      <c r="T20" s="528" t="n"/>
+      <c r="O20" s="529" t="n"/>
+      <c r="P20" s="529" t="n"/>
+      <c r="Q20" s="529" t="n"/>
+      <c r="R20" s="529" t="n"/>
+      <c r="S20" s="529" t="n"/>
+      <c r="T20" s="529" t="n"/>
     </row>
     <row r="21" ht="27" customHeight="1">
       <c r="A21" s="520" t="n"/>
@@ -11374,12 +11583,12 @@
       <c r="L21" s="13" t="n"/>
       <c r="M21" s="13" t="n"/>
       <c r="N21" s="13" t="n"/>
-      <c r="O21" s="528" t="n"/>
-      <c r="P21" s="528" t="n"/>
-      <c r="Q21" s="528" t="n"/>
-      <c r="R21" s="528" t="n"/>
-      <c r="S21" s="528" t="n"/>
-      <c r="T21" s="528" t="n"/>
+      <c r="O21" s="529" t="n"/>
+      <c r="P21" s="529" t="n"/>
+      <c r="Q21" s="529" t="n"/>
+      <c r="R21" s="529" t="n"/>
+      <c r="S21" s="529" t="n"/>
+      <c r="T21" s="529" t="n"/>
     </row>
     <row r="22" ht="27" customHeight="1">
       <c r="A22" s="520" t="n"/>
@@ -11396,12 +11605,12 @@
       <c r="L22" s="13" t="n"/>
       <c r="M22" s="13" t="n"/>
       <c r="N22" s="13" t="n"/>
-      <c r="O22" s="528" t="n"/>
-      <c r="P22" s="528" t="n"/>
-      <c r="Q22" s="528" t="n"/>
-      <c r="R22" s="528" t="n"/>
-      <c r="S22" s="528" t="n"/>
-      <c r="T22" s="528" t="n"/>
+      <c r="O22" s="529" t="n"/>
+      <c r="P22" s="529" t="n"/>
+      <c r="Q22" s="529" t="n"/>
+      <c r="R22" s="529" t="n"/>
+      <c r="S22" s="529" t="n"/>
+      <c r="T22" s="529" t="n"/>
     </row>
     <row r="23" ht="27" customHeight="1">
       <c r="A23" s="520" t="n"/>
@@ -11418,12 +11627,12 @@
       <c r="L23" s="13" t="n"/>
       <c r="M23" s="13" t="n"/>
       <c r="N23" s="13" t="n"/>
-      <c r="O23" s="528" t="n"/>
-      <c r="P23" s="528" t="n"/>
-      <c r="Q23" s="528" t="n"/>
-      <c r="R23" s="528" t="n"/>
-      <c r="S23" s="528" t="n"/>
-      <c r="T23" s="528" t="n"/>
+      <c r="O23" s="529" t="n"/>
+      <c r="P23" s="529" t="n"/>
+      <c r="Q23" s="529" t="n"/>
+      <c r="R23" s="529" t="n"/>
+      <c r="S23" s="529" t="n"/>
+      <c r="T23" s="529" t="n"/>
     </row>
     <row r="24" ht="27" customHeight="1">
       <c r="A24" s="520" t="n"/>
@@ -11440,12 +11649,12 @@
       <c r="L24" s="13" t="n"/>
       <c r="M24" s="13" t="n"/>
       <c r="N24" s="13" t="n"/>
-      <c r="O24" s="528" t="n"/>
-      <c r="P24" s="528" t="n"/>
-      <c r="Q24" s="528" t="n"/>
-      <c r="R24" s="528" t="n"/>
-      <c r="S24" s="528" t="n"/>
-      <c r="T24" s="528" t="n"/>
+      <c r="O24" s="529" t="n"/>
+      <c r="P24" s="529" t="n"/>
+      <c r="Q24" s="529" t="n"/>
+      <c r="R24" s="529" t="n"/>
+      <c r="S24" s="529" t="n"/>
+      <c r="T24" s="529" t="n"/>
     </row>
     <row r="25" ht="27" customHeight="1">
       <c r="A25" s="520" t="n"/>
@@ -11478,12 +11687,12 @@
       <c r="L26" s="13" t="n"/>
       <c r="M26" s="13" t="n"/>
       <c r="N26" s="13" t="n"/>
-      <c r="O26" s="528" t="n"/>
-      <c r="P26" s="528" t="n"/>
-      <c r="Q26" s="528" t="n"/>
-      <c r="R26" s="528" t="n"/>
-      <c r="S26" s="528" t="n"/>
-      <c r="T26" s="528" t="n"/>
+      <c r="O26" s="529" t="n"/>
+      <c r="P26" s="529" t="n"/>
+      <c r="Q26" s="529" t="n"/>
+      <c r="R26" s="529" t="n"/>
+      <c r="S26" s="529" t="n"/>
+      <c r="T26" s="529" t="n"/>
     </row>
     <row r="27" ht="27" customHeight="1">
       <c r="A27" s="520" t="n"/>
@@ -11500,12 +11709,12 @@
       <c r="L27" s="13" t="n"/>
       <c r="M27" s="13" t="n"/>
       <c r="N27" s="13" t="n"/>
-      <c r="O27" s="528" t="n"/>
-      <c r="P27" s="528" t="n"/>
-      <c r="Q27" s="528" t="n"/>
-      <c r="R27" s="528" t="n"/>
-      <c r="S27" s="528" t="n"/>
-      <c r="T27" s="528" t="n"/>
+      <c r="O27" s="529" t="n"/>
+      <c r="P27" s="529" t="n"/>
+      <c r="Q27" s="529" t="n"/>
+      <c r="R27" s="529" t="n"/>
+      <c r="S27" s="529" t="n"/>
+      <c r="T27" s="529" t="n"/>
     </row>
     <row r="28" ht="27" customHeight="1">
       <c r="A28" s="520" t="n"/>
@@ -11522,12 +11731,12 @@
       <c r="L28" s="13" t="n"/>
       <c r="M28" s="13" t="n"/>
       <c r="N28" s="13" t="n"/>
-      <c r="O28" s="528" t="n"/>
-      <c r="P28" s="528" t="n"/>
-      <c r="Q28" s="528" t="n"/>
-      <c r="R28" s="528" t="n"/>
-      <c r="S28" s="528" t="n"/>
-      <c r="T28" s="528" t="n"/>
+      <c r="O28" s="529" t="n"/>
+      <c r="P28" s="529" t="n"/>
+      <c r="Q28" s="529" t="n"/>
+      <c r="R28" s="529" t="n"/>
+      <c r="S28" s="529" t="n"/>
+      <c r="T28" s="529" t="n"/>
     </row>
     <row r="29" ht="27" customHeight="1">
       <c r="A29" s="520" t="n"/>
@@ -11544,12 +11753,12 @@
       <c r="L29" s="13" t="n"/>
       <c r="M29" s="13" t="n"/>
       <c r="N29" s="13" t="n"/>
-      <c r="O29" s="528" t="n"/>
-      <c r="P29" s="528" t="n"/>
-      <c r="Q29" s="528" t="n"/>
-      <c r="R29" s="528" t="n"/>
-      <c r="S29" s="528" t="n"/>
-      <c r="T29" s="528" t="n"/>
+      <c r="O29" s="529" t="n"/>
+      <c r="P29" s="529" t="n"/>
+      <c r="Q29" s="529" t="n"/>
+      <c r="R29" s="529" t="n"/>
+      <c r="S29" s="529" t="n"/>
+      <c r="T29" s="529" t="n"/>
     </row>
     <row r="30" ht="27" customHeight="1">
       <c r="A30" s="520" t="n"/>
@@ -11566,12 +11775,12 @@
       <c r="L30" s="13" t="n"/>
       <c r="M30" s="13" t="n"/>
       <c r="N30" s="13" t="n"/>
-      <c r="O30" s="528" t="n"/>
-      <c r="P30" s="528" t="n"/>
-      <c r="Q30" s="528" t="n"/>
-      <c r="R30" s="528" t="n"/>
-      <c r="S30" s="528" t="n"/>
-      <c r="T30" s="528" t="n"/>
+      <c r="O30" s="529" t="n"/>
+      <c r="P30" s="529" t="n"/>
+      <c r="Q30" s="529" t="n"/>
+      <c r="R30" s="529" t="n"/>
+      <c r="S30" s="529" t="n"/>
+      <c r="T30" s="529" t="n"/>
     </row>
     <row r="31" ht="27" customHeight="1">
       <c r="A31" s="520" t="n"/>
@@ -11588,12 +11797,12 @@
       <c r="L31" s="13" t="n"/>
       <c r="M31" s="13" t="n"/>
       <c r="N31" s="13" t="n"/>
-      <c r="O31" s="528" t="n"/>
-      <c r="P31" s="528" t="n"/>
-      <c r="Q31" s="528" t="n"/>
-      <c r="R31" s="528" t="n"/>
-      <c r="S31" s="528" t="n"/>
-      <c r="T31" s="528" t="n"/>
+      <c r="O31" s="529" t="n"/>
+      <c r="P31" s="529" t="n"/>
+      <c r="Q31" s="529" t="n"/>
+      <c r="R31" s="529" t="n"/>
+      <c r="S31" s="529" t="n"/>
+      <c r="T31" s="529" t="n"/>
     </row>
     <row r="32" ht="27" customHeight="1">
       <c r="A32" s="520" t="n"/>
@@ -11610,12 +11819,12 @@
       <c r="L32" s="13" t="n"/>
       <c r="M32" s="13" t="n"/>
       <c r="N32" s="13" t="n"/>
-      <c r="O32" s="528" t="n"/>
-      <c r="P32" s="528" t="n"/>
-      <c r="Q32" s="528" t="n"/>
-      <c r="R32" s="528" t="n"/>
-      <c r="S32" s="528" t="n"/>
-      <c r="T32" s="528" t="n"/>
+      <c r="O32" s="529" t="n"/>
+      <c r="P32" s="529" t="n"/>
+      <c r="Q32" s="529" t="n"/>
+      <c r="R32" s="529" t="n"/>
+      <c r="S32" s="529" t="n"/>
+      <c r="T32" s="529" t="n"/>
     </row>
     <row r="33" ht="27" customHeight="1">
       <c r="A33" s="521" t="n"/>
@@ -11632,12 +11841,12 @@
       <c r="L33" s="13" t="n"/>
       <c r="M33" s="13" t="n"/>
       <c r="N33" s="13" t="n"/>
-      <c r="O33" s="528" t="n"/>
-      <c r="P33" s="528" t="n"/>
-      <c r="Q33" s="528" t="n"/>
-      <c r="R33" s="528" t="n"/>
-      <c r="S33" s="528" t="n"/>
-      <c r="T33" s="528" t="n"/>
+      <c r="O33" s="529" t="n"/>
+      <c r="P33" s="529" t="n"/>
+      <c r="Q33" s="529" t="n"/>
+      <c r="R33" s="529" t="n"/>
+      <c r="S33" s="529" t="n"/>
+      <c r="T33" s="529" t="n"/>
     </row>
     <row r="34" ht="27" customHeight="1">
       <c r="A34" s="520" t="n"/>
@@ -11654,12 +11863,12 @@
       <c r="L34" s="13" t="n"/>
       <c r="M34" s="13" t="n"/>
       <c r="N34" s="13" t="n"/>
-      <c r="O34" s="528" t="n"/>
-      <c r="P34" s="528" t="n"/>
-      <c r="Q34" s="528" t="n"/>
-      <c r="R34" s="528" t="n"/>
-      <c r="S34" s="528" t="n"/>
-      <c r="T34" s="528" t="n"/>
+      <c r="O34" s="529" t="n"/>
+      <c r="P34" s="529" t="n"/>
+      <c r="Q34" s="529" t="n"/>
+      <c r="R34" s="529" t="n"/>
+      <c r="S34" s="529" t="n"/>
+      <c r="T34" s="529" t="n"/>
     </row>
     <row r="35" ht="27" customHeight="1">
       <c r="A35" s="519" t="n"/>
@@ -11676,12 +11885,12 @@
       <c r="L35" s="13" t="n"/>
       <c r="M35" s="13" t="n"/>
       <c r="N35" s="13" t="n"/>
-      <c r="O35" s="528" t="n"/>
-      <c r="P35" s="528" t="n"/>
-      <c r="Q35" s="528" t="n"/>
-      <c r="R35" s="528" t="n"/>
-      <c r="S35" s="528" t="n"/>
-      <c r="T35" s="528" t="n"/>
+      <c r="O35" s="529" t="n"/>
+      <c r="P35" s="529" t="n"/>
+      <c r="Q35" s="529" t="n"/>
+      <c r="R35" s="529" t="n"/>
+      <c r="S35" s="529" t="n"/>
+      <c r="T35" s="529" t="n"/>
     </row>
     <row r="36" ht="27" customHeight="1" thickBot="1">
       <c r="A36" s="522" t="n"/>
@@ -11698,23 +11907,23 @@
       <c r="L36" s="13" t="n"/>
       <c r="M36" s="13" t="n"/>
       <c r="N36" s="13" t="n"/>
-      <c r="O36" s="528" t="n"/>
-      <c r="P36" s="528" t="n"/>
-      <c r="Q36" s="528" t="n"/>
-      <c r="R36" s="528" t="n"/>
-      <c r="S36" s="528" t="n"/>
-      <c r="T36" s="528" t="n"/>
+      <c r="O36" s="529" t="n"/>
+      <c r="P36" s="529" t="n"/>
+      <c r="Q36" s="529" t="n"/>
+      <c r="R36" s="529" t="n"/>
+      <c r="S36" s="529" t="n"/>
+      <c r="T36" s="529" t="n"/>
     </row>
     <row r="37" ht="27" customHeight="1">
-      <c r="A37" s="528" t="n"/>
-      <c r="B37" s="528" t="n"/>
+      <c r="A37" s="529" t="n"/>
+      <c r="B37" s="529" t="n"/>
       <c r="C37" s="18" t="n"/>
-      <c r="D37" s="528" t="n"/>
-      <c r="E37" s="528" t="n"/>
-      <c r="F37" s="528" t="n"/>
+      <c r="D37" s="529" t="n"/>
+      <c r="E37" s="529" t="n"/>
+      <c r="F37" s="529" t="n"/>
       <c r="G37" s="22" t="n"/>
-      <c r="H37" s="528" t="n"/>
-      <c r="I37" s="528" t="n"/>
+      <c r="H37" s="529" t="n"/>
+      <c r="I37" s="529" t="n"/>
       <c r="J37" s="119" t="n"/>
       <c r="K37" s="119" t="n"/>
       <c r="L37" s="119" t="n"/>
@@ -11722,7 +11931,7 @@
       <c r="N37" s="119" t="n"/>
     </row>
     <row r="38" ht="27" customHeight="1">
-      <c r="A38" s="528" t="inlineStr">
+      <c r="A38" s="529" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -11732,33 +11941,33 @@
         <v/>
       </c>
       <c r="C38" s="18" t="n"/>
-      <c r="D38" s="528" t="n"/>
-      <c r="E38" s="528" t="n"/>
-      <c r="F38" s="528" t="n"/>
+      <c r="D38" s="529" t="n"/>
+      <c r="E38" s="529" t="n"/>
+      <c r="F38" s="529" t="n"/>
       <c r="G38" s="22" t="n"/>
-      <c r="H38" s="528" t="n"/>
-      <c r="I38" s="528" t="n"/>
-      <c r="J38" s="528" t="n"/>
-      <c r="K38" s="528" t="n"/>
-      <c r="L38" s="528" t="n"/>
-      <c r="M38" s="528" t="n"/>
-      <c r="N38" s="528" t="n"/>
+      <c r="H38" s="529" t="n"/>
+      <c r="I38" s="529" t="n"/>
+      <c r="J38" s="529" t="n"/>
+      <c r="K38" s="529" t="n"/>
+      <c r="L38" s="529" t="n"/>
+      <c r="M38" s="529" t="n"/>
+      <c r="N38" s="529" t="n"/>
     </row>
     <row r="39" ht="27" customHeight="1">
-      <c r="A39" s="528" t="n"/>
-      <c r="B39" s="528" t="n"/>
+      <c r="A39" s="529" t="n"/>
+      <c r="B39" s="529" t="n"/>
       <c r="C39" s="18" t="n"/>
-      <c r="D39" s="528" t="n"/>
-      <c r="E39" s="528" t="n"/>
-      <c r="F39" s="528" t="n"/>
+      <c r="D39" s="529" t="n"/>
+      <c r="E39" s="529" t="n"/>
+      <c r="F39" s="529" t="n"/>
       <c r="G39" s="22" t="n"/>
-      <c r="H39" s="528" t="n"/>
-      <c r="I39" s="528" t="n"/>
-      <c r="J39" s="528" t="n"/>
-      <c r="K39" s="528" t="n"/>
-      <c r="L39" s="528" t="n"/>
-      <c r="M39" s="528" t="n"/>
-      <c r="N39" s="528" t="n"/>
+      <c r="H39" s="529" t="n"/>
+      <c r="I39" s="529" t="n"/>
+      <c r="J39" s="529" t="n"/>
+      <c r="K39" s="529" t="n"/>
+      <c r="L39" s="529" t="n"/>
+      <c r="M39" s="529" t="n"/>
+      <c r="N39" s="529" t="n"/>
     </row>
     <row r="40" ht="16" customHeight="1">
       <c r="G40" s="22" t="n"/>

</xml_diff>